<commit_message>
Take 5 everyone. (melody only)
</commit_message>
<xml_diff>
--- a/FrequencyChart.xlsx
+++ b/FrequencyChart.xlsx
@@ -4507,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection sqref="A1:A109"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>